<commit_message>
New version of EPPlus. Minor changes for the documentation. New Icon.
</commit_message>
<xml_diff>
--- a/Data/ExcelReadWrite.xlsx
+++ b/Data/ExcelReadWrite.xlsx
@@ -1,25 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22508"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22513"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\(svn azure)\SimioCloud\Github\ExcelGridDataProviderEPPlus\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A20C21E0-E4DE-4DF5-AA4D-9D9C7C2F4573}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5821564F-0259-4E27-8DC6-7A07EF57E236}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2184" yWindow="1980" windowWidth="17280" windowHeight="10056" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="58080" yWindow="480" windowWidth="21600" windowHeight="12675" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Simple Data" sheetId="1" r:id="rId1"/>
     <sheet name="Empty Sheet" sheetId="5" r:id="rId2"/>
     <sheet name="Sparse Data" sheetId="2" r:id="rId3"/>
-    <sheet name="Table" sheetId="3" r:id="rId4"/>
+    <sheet name="OrderTable" sheetId="3" r:id="rId4"/>
     <sheet name="Named Ranges" sheetId="4" r:id="rId5"/>
   </sheets>
   <definedNames>
+    <definedName name="DatesAndNumbers">'Named Ranges'!$B$26:$G$30</definedName>
+    <definedName name="ExcelFormatRange">'Named Ranges'!$B$34:$E$38</definedName>
+    <definedName name="ExcelFormats">'Named Ranges'!$B$34:$E$41</definedName>
     <definedName name="MyNamedRange">'Named Ranges'!$B$4:$E$8</definedName>
     <definedName name="NamedRange2">'Named Ranges'!$B$15:$E$19</definedName>
     <definedName name="OrderDate" localSheetId="3">Table1[#All]</definedName>
@@ -40,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="69">
   <si>
     <t>ColumnA</t>
   </si>
@@ -166,15 +169,99 @@
   </si>
   <si>
     <t>MyString</t>
+  </si>
+  <si>
+    <t>DateAsText</t>
+  </si>
+  <si>
+    <t>DateAsDate</t>
+  </si>
+  <si>
+    <t>Number</t>
+  </si>
+  <si>
+    <t>NumberLocalized</t>
+  </si>
+  <si>
+    <t>12/1/2020</t>
+  </si>
+  <si>
+    <t>12/1/2020 13:14</t>
+  </si>
+  <si>
+    <t>12/13/1905</t>
+  </si>
+  <si>
+    <t>12/13/1970 13:14</t>
+  </si>
+  <si>
+    <t>1,234.00</t>
+  </si>
+  <si>
+    <t>DateLocalized</t>
+  </si>
+  <si>
+    <t>NumberAsText</t>
+  </si>
+  <si>
+    <t>NumberAsNumber</t>
+  </si>
+  <si>
+    <t>Boolean</t>
+  </si>
+  <si>
+    <t>Text</t>
+  </si>
+  <si>
+    <t>This range (ExcelFormats) has values for each basic type with various Excel Formatting)</t>
+  </si>
+  <si>
+    <t>12/22/1905 5am</t>
+  </si>
+  <si>
+    <t>The</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>Has</t>
+  </si>
+  <si>
+    <t>Come</t>
+  </si>
+  <si>
+    <t>Walrus</t>
+  </si>
+  <si>
+    <t>Said</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>false</t>
+  </si>
+  <si>
+    <t>True</t>
+  </si>
+  <si>
+    <t>False</t>
+  </si>
+  <si>
+    <t>DateTime</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="5">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="m/d/yy;@"/>
+    <numFmt numFmtId="167" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="169" formatCode="0.0000E+00"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -213,7 +300,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -245,6 +332,17 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="12" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -602,7 +700,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -1281,8 +1379,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B4:H47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2313,16 +2411,13 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAFCD98A-2DBD-4CE7-BB13-0E9F19908232}">
-  <dimension ref="B4:H19"/>
+  <dimension ref="A4:H41"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="2" max="5" width="12.33203125" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="18.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="4" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
@@ -2428,7 +2523,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B17">
         <v>21</v>
       </c>
@@ -2442,7 +2537,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B18">
         <v>31</v>
       </c>
@@ -2456,7 +2551,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B19">
         <v>41</v>
       </c>
@@ -2468,6 +2563,268 @@
       </c>
       <c r="E19" t="s">
         <v>36</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>0</v>
+      </c>
+      <c r="B26" t="s">
+        <v>43</v>
+      </c>
+      <c r="C26" t="s">
+        <v>42</v>
+      </c>
+      <c r="D26" t="s">
+        <v>51</v>
+      </c>
+      <c r="E26" t="s">
+        <v>52</v>
+      </c>
+      <c r="F26" t="s">
+        <v>53</v>
+      </c>
+      <c r="G26" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>1</v>
+      </c>
+      <c r="B27" s="10">
+        <v>44166</v>
+      </c>
+      <c r="C27" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="D27" s="10">
+        <v>44166</v>
+      </c>
+      <c r="E27" s="12">
+        <v>123</v>
+      </c>
+      <c r="F27" s="14">
+        <v>123</v>
+      </c>
+      <c r="G27" s="16">
+        <v>123450</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>2</v>
+      </c>
+      <c r="B28" s="11">
+        <v>44166.551388888889</v>
+      </c>
+      <c r="C28" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="D28" s="11">
+        <v>44166.551388888889</v>
+      </c>
+      <c r="E28" s="12">
+        <v>12.34</v>
+      </c>
+      <c r="F28" s="14">
+        <v>12.34</v>
+      </c>
+      <c r="G28" s="14">
+        <v>12.34</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>3</v>
+      </c>
+      <c r="B29" s="10">
+        <v>2174</v>
+      </c>
+      <c r="C29" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="D29" s="10">
+        <v>2174</v>
+      </c>
+      <c r="E29" s="12">
+        <v>123.45</v>
+      </c>
+      <c r="F29" s="13">
+        <v>123.45</v>
+      </c>
+      <c r="G29" s="13">
+        <v>123.45</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>4</v>
+      </c>
+      <c r="B30" s="11">
+        <v>25915.551388888889</v>
+      </c>
+      <c r="C30" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="D30" s="11">
+        <v>25915.551388888889</v>
+      </c>
+      <c r="E30" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="F30" s="17">
+        <v>1234</v>
+      </c>
+      <c r="G30" s="14" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B33" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>0</v>
+      </c>
+      <c r="B34" t="s">
+        <v>68</v>
+      </c>
+      <c r="C34" t="s">
+        <v>44</v>
+      </c>
+      <c r="D34" t="s">
+        <v>54</v>
+      </c>
+      <c r="E34" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>1</v>
+      </c>
+      <c r="B35" s="10">
+        <v>43861</v>
+      </c>
+      <c r="C35">
+        <v>123.45</v>
+      </c>
+      <c r="D35" t="b">
+        <v>1</v>
+      </c>
+      <c r="E35" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>2</v>
+      </c>
+      <c r="B36" s="11">
+        <v>43861.529861111114</v>
+      </c>
+      <c r="C36" s="14">
+        <v>123.45</v>
+      </c>
+      <c r="D36" t="b">
+        <v>0</v>
+      </c>
+      <c r="E36" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>3</v>
+      </c>
+      <c r="B37" t="s">
+        <v>57</v>
+      </c>
+      <c r="C37" s="17">
+        <v>123.45</v>
+      </c>
+      <c r="D37" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="E37" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>4</v>
+      </c>
+      <c r="B38" s="18">
+        <v>43956</v>
+      </c>
+      <c r="C38" s="19">
+        <v>123.45</v>
+      </c>
+      <c r="D38" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="E38" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>5</v>
+      </c>
+      <c r="B39" s="11">
+        <v>25705.3125</v>
+      </c>
+      <c r="C39" s="20">
+        <v>123.45</v>
+      </c>
+      <c r="D39" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="E39" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>6</v>
+      </c>
+      <c r="B40" s="10">
+        <v>25705</v>
+      </c>
+      <c r="C40" s="15">
+        <f>12345/9</f>
+        <v>1371.6666666666667</v>
+      </c>
+      <c r="D40" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="E40" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>7</v>
+      </c>
+      <c r="B41" s="11">
+        <v>28611.65625</v>
+      </c>
+      <c r="C41" s="21">
+        <v>123.45</v>
+      </c>
+      <c r="D41" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="E41" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>